<commit_message>
excel file has been updated
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Python\git-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Python\gitpurpose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{33C182A0-BBE8-4EFE-A67E-F0D88BA6F705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8136B7-2A50-4D40-BE2F-153569AFD46D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -45,11 +45,14 @@
   <si>
     <t>183 cm</t>
   </si>
+  <si>
+    <t>188 cm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,11 +892,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +948,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>